<commit_message>
Rediseño de base de datos 0.1
En esta versión empiezo a cambiar la base de datos, para usar Firebase
</commit_message>
<xml_diff>
--- a/cogs/idiomas.xlsx
+++ b/cogs/idiomas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\bot python\cogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CA56D5-581E-4B5D-9A0F-0908A5B25170}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D12594-A683-4D6E-ACE0-DF26EA354A7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DE6446BD-563B-4FC6-AA1A-933AD8BD7CBF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="193">
   <si>
     <t>Español</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Tu personaje ha sido iniciado con éxito.</t>
   </si>
   <si>
-    <t>Aún no has creado un personaje, usa `rpg&gt;empezar` para hacerlo.</t>
-  </si>
-  <si>
     <t>Inventario</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>I have deleted `{cant} messages`.</t>
   </si>
   <si>
-    <t>You must put the number of messages you want to delete `rpg&gt;clear &lt;num&gt;` and the number must be greater than 0.</t>
-  </si>
-  <si>
     <t>You do not have permission to use this command.</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>Game commands are disabled for this channel.</t>
   </si>
   <si>
-    <t>You haven't created a character yet, use `rpg&gt; start` to do it.</t>
-  </si>
-  <si>
     <t>Inventory</t>
   </si>
   <si>
@@ -210,15 +201,6 @@
     <t>Armadura básica</t>
   </si>
   <si>
-    <t>Sube 10 puntos de vida.</t>
-  </si>
-  <si>
-    <t>Sube 20 puntos de vida.</t>
-  </si>
-  <si>
-    <t>Úsalo mientras estés luchando, harás un ataque de fuego.</t>
-  </si>
-  <si>
     <t>Únelo con otros objetos, tal vez consigas hacer algo.</t>
   </si>
   <si>
@@ -243,9 +225,6 @@
     <t>Recover 20 HP points.</t>
   </si>
   <si>
-    <t>Use it while you are fighting, you will make a fire attack.</t>
-  </si>
-  <si>
     <t>Join it with other objects, maybe you can get something done.</t>
   </si>
   <si>
@@ -276,9 +255,6 @@
     <t>The number of messages must be less than or equal to 300.</t>
   </si>
   <si>
-    <t>failed to hit you.</t>
-  </si>
-  <si>
     <t>Your character has been successfully started.</t>
   </si>
   <si>
@@ -291,12 +267,6 @@
     <t>You're already fighting something.</t>
   </si>
   <si>
-    <t>No tienes puntos de vida, usa `rpg&gt;descansar` para recuperar toda tu vida.</t>
-  </si>
-  <si>
-    <t>You have no hp, use `rpg&gt; rest` to get your whole hp back.</t>
-  </si>
-  <si>
     <t>Bosque</t>
   </si>
   <si>
@@ -351,13 +321,301 @@
     <t>Apparently the channel that was being used to carry out your fight has been deleted.</t>
   </si>
   <si>
-    <t>Debes poner la cantidad de mensajes que quieras borrar `rpg&gt;clear &lt;num&gt;` y el número debe ser mayor a 0 y no mayor a 300.</t>
-  </si>
-  <si>
     <t>aparece.</t>
   </si>
   <si>
     <t>appears.</t>
+  </si>
+  <si>
+    <t>Debes mencionar a la persona que quieres silenciar `c!mute &lt;persona&gt; &lt;razón : opcional&gt;`.</t>
+  </si>
+  <si>
+    <t>Debes poner la cantidad de mensajes que quieras borrar `c!clear &lt;num&gt;` y el número debe ser mayor a 0 y no mayor a 300.</t>
+  </si>
+  <si>
+    <t>Aún no has creado un personaje, usa `c!empezar` para hacerlo.</t>
+  </si>
+  <si>
+    <t>You haven't created a character yet, use `c! start` to do it.</t>
+  </si>
+  <si>
+    <t>No tienes puntos de vida, usa `c!descansar` para recuperar toda tu vida.</t>
+  </si>
+  <si>
+    <t>You have no hp, use `c! rest` to get your whole hp back.</t>
+  </si>
+  <si>
+    <t>You must mention the person you want to mute `c!mute &lt;person&gt; &lt;reason : optional&gt;`.</t>
+  </si>
+  <si>
+    <t>Português</t>
+  </si>
+  <si>
+    <t>Você não pode usar esse comando neste canal.</t>
+  </si>
+  <si>
+    <t>Eu apaguei `1 mensagem`.</t>
+  </si>
+  <si>
+    <t>Eu apaguei `{cant} mensagems`.</t>
+  </si>
+  <si>
+    <t>You must put the number of messages you want to delete `c!clear &lt;num&gt;` and the number must be greater than 0 and not greater than 300.</t>
+  </si>
+  <si>
+    <t>Você deve colocar o número de mensagens que deseja apagar `c!clear &lt;num&gt;` e o número deve ser maior que 0 e não maior que 300.</t>
+  </si>
+  <si>
+    <t>Você não tem permissão para usar este comando.</t>
+  </si>
+  <si>
+    <t>Comando inexistente.</t>
+  </si>
+  <si>
+    <t>Common Armor{salto}Defense: {def}</t>
+  </si>
+  <si>
+    <t>Você está lutando contra</t>
+  </si>
+  <si>
+    <t>No especificada.</t>
+  </si>
+  <si>
+    <t>Not specified.</t>
+  </si>
+  <si>
+    <t>Não especificada.</t>
+  </si>
+  <si>
+    <t>Você perdeu contra</t>
+  </si>
+  <si>
+    <t>Seu HP</t>
+  </si>
+  <si>
+    <t>pontos</t>
+  </si>
+  <si>
+    <t>ponto</t>
+  </si>
+  <si>
+    <t>your attack has failed.</t>
+  </si>
+  <si>
+    <t>seu ataque falhou.</t>
+  </si>
+  <si>
+    <t>Seu personagem já existe, se você quiser reiniciá-lo, no momento você não pode.</t>
+  </si>
+  <si>
+    <t>Seu personagem foi iniciado com sucesso.</t>
+  </si>
+  <si>
+    <t>Os comandos de jogo estão desabilitados para este canal.</t>
+  </si>
+  <si>
+    <t>Você ainda não criou um personagem, use `c!start` para fazê-lo.</t>
+  </si>
+  <si>
+    <t>Inventário</t>
+  </si>
+  <si>
+    <t>Nenhum</t>
+  </si>
+  <si>
+    <t>Estatisticas</t>
+  </si>
+  <si>
+    <t>Nível</t>
+  </si>
+  <si>
+    <t>Defesa</t>
+  </si>
+  <si>
+    <t>Arma equipada</t>
+  </si>
+  <si>
+    <t>Armadura equipada</t>
+  </si>
+  <si>
+    <t>Próximo nível</t>
+  </si>
+  <si>
+    <t>Dinheiro</t>
+  </si>
+  <si>
+    <t>O número de mensagens deve ser menor ou igual a 300.</t>
+  </si>
+  <si>
+    <t>Você já está lutando contra algo.</t>
+  </si>
+  <si>
+    <t>Você não tem pontos de vida, use `c!descansar` para ter toda a sua vida de volta.</t>
+  </si>
+  <si>
+    <t>Áreas que você pode explorar:</t>
+  </si>
+  <si>
+    <t>Você perdeu sua mensagem de luta?</t>
+  </si>
+  <si>
+    <t>Você não pode fazer isso no meio de uma luta.</t>
+  </si>
+  <si>
+    <t>Sua vida foi recuperada com sucesso.</t>
+  </si>
+  <si>
+    <t>Um erro ocorreu. Não foi possível processar sua luta.</t>
+  </si>
+  <si>
+    <t>Aparentemente, o canal que estava sendo usado para realizar sua luta foi removido.</t>
+  </si>
+  <si>
+    <t>Parece</t>
+  </si>
+  <si>
+    <t>Você deve mencionar a pessoa que deseja silenciar `c!mute &lt;pessoa&gt; &lt;razão: opcional&gt;`.</t>
+  </si>
+  <si>
+    <t>Floresta</t>
+  </si>
+  <si>
+    <t>Cogumelo</t>
+  </si>
+  <si>
+    <t>Saliva</t>
+  </si>
+  <si>
+    <t>Cenoura</t>
+  </si>
+  <si>
+    <t>Pó de fada</t>
+  </si>
+  <si>
+    <t>Espada básica</t>
+  </si>
+  <si>
+    <t>Armadura básica</t>
+  </si>
+  <si>
+    <t>Recupera 10 puntos de vida.</t>
+  </si>
+  <si>
+    <t>Recupera 10 pontos de vida.</t>
+  </si>
+  <si>
+    <t>Junte-o a outros objetos, talvez você consiga fazer algo.</t>
+  </si>
+  <si>
+    <t>Recupera 20 puntos de vida.</t>
+  </si>
+  <si>
+    <t>Recupera 20 pontos de vida.</t>
+  </si>
+  <si>
+    <t>Úsalo mientras estés luchando, harás un ataque de fuego.{salto}Ataque: 10</t>
+  </si>
+  <si>
+    <t>Use it while you are fighting, you will make a fire attack.{salto}Attack: 10</t>
+  </si>
+  <si>
+    <t>Use-o enquanto estiver lutando, você fará um ataque de fogo.{salto}Ataque: 10</t>
+  </si>
+  <si>
+    <t>Espada básica{salto}Ataque: {atq}{salto}Precisão: {prec}</t>
+  </si>
+  <si>
+    <t>Armadura básica{salto}Defensa: {def}</t>
+  </si>
+  <si>
+    <t>Fada</t>
+  </si>
+  <si>
+    <t>No puedes silenciar a un administrador.</t>
+  </si>
+  <si>
+    <t>You cannot mute an administrator.</t>
+  </si>
+  <si>
+    <t>Você não pode silenciar um administrador</t>
+  </si>
+  <si>
+    <t>Para silenciar a un moderador tienes que tener permisos de administrador.</t>
+  </si>
+  <si>
+    <t>Para silenciar um moderador, você deve ter direitos de administrador.</t>
+  </si>
+  <si>
+    <t>To mute a moderator you must have administrator rights.</t>
+  </si>
+  <si>
+    <t>La palabra ||{palabra}|| está prohibida en este server.</t>
+  </si>
+  <si>
+    <t>The word ||{palabra}|| is forbidden on this server.</t>
+  </si>
+  <si>
+    <t>A palavra ||{palabra}|| é proibida neste servidor.</t>
+  </si>
+  <si>
+    <t>Moderador</t>
+  </si>
+  <si>
+    <t>Moderator</t>
+  </si>
+  <si>
+    <t>Silenciado</t>
+  </si>
+  <si>
+    <t>Muted</t>
+  </si>
+  <si>
+    <t>Fue silenciado por:</t>
+  </si>
+  <si>
+    <t>Foi silenciado por:</t>
+  </si>
+  <si>
+    <t>Usuario:</t>
+  </si>
+  <si>
+    <t>User:</t>
+  </si>
+  <si>
+    <t>Was silenced by:</t>
+  </si>
+  <si>
+    <t>Reason:</t>
+  </si>
+  <si>
+    <t>Razón:</t>
+  </si>
+  <si>
+    <t>Razão:</t>
+  </si>
+  <si>
+    <t>Warned</t>
+  </si>
+  <si>
+    <t>Avisado</t>
+  </si>
+  <si>
+    <t>Fue avisado por:</t>
+  </si>
+  <si>
+    <t>Was warned by:</t>
+  </si>
+  <si>
+    <t>Foi avisado por:</t>
+  </si>
+  <si>
+    <t>Haber sido avisado {cant} veces en menos de {tiempo} {medida}.</t>
+  </si>
+  <si>
+    <t>Having been warned {cant} times in less than {tiempo} {medida}.</t>
+  </si>
+  <si>
+    <t>Ter sido avisado {cant} vezes em menos de {tiempo} {medida}.</t>
   </si>
 </sst>
 </file>
@@ -414,7 +672,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -424,9 +682,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -743,26 +998,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECE8E95-8ADA-4BBB-8313-6E88F6DAFB67}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="50.7109375" style="2" customWidth="1"/>
+    <col min="2" max="4" width="50.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -770,10 +1028,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -781,10 +1042,13 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -792,21 +1056,27 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -814,10 +1084,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -825,21 +1098,27 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -847,10 +1126,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -858,10 +1140,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -869,10 +1154,13 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -880,10 +1168,13 @@
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -891,10 +1182,13 @@
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -902,10 +1196,13 @@
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -913,10 +1210,13 @@
         <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -924,260 +1224,514 @@
         <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>106</v>
+        <v>95</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -1188,34 +1742,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87296DC2-339E-40B3-8D1B-F1751A8F576E}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="50.7109375" style="4" customWidth="1"/>
+    <col min="2" max="4" width="50.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>87</v>
+      <c r="B2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1225,100 +1785,125 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36086715-9A10-4B62-9A26-AE32487930A2}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="50.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1329,97 +1914,124 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171B6A99-3D9B-42F3-8D34-8FFC4557EF39}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="50.7109375" style="3" customWidth="1"/>
+    <col min="2" max="4" width="50.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>57</v>
+        <v>153</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>156</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>59</v>
+        <v>158</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1429,45 +2041,54 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9572496D-EE77-4B6C-AC88-9EA6DD028EAC}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="50.7109375" customWidth="1"/>
+    <col min="2" max="4" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rediseño de base de datos 0.2
Sigo adaptando el código para que funcione con Firebase
</commit_message>
<xml_diff>
--- a/cogs/idiomas.xlsx
+++ b/cogs/idiomas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\bot python\cogs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Proyecto bot de Discord\Codigo\cogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D12594-A683-4D6E-ACE0-DF26EA354A7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60266F42-2E24-4B06-9B56-500F238FDDA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DE6446BD-563B-4FC6-AA1A-933AD8BD7CBF}"/>
   </bookViews>
@@ -16,8 +16,13 @@
     <sheet name="bot" sheetId="1" r:id="rId1"/>
     <sheet name="areas" sheetId="5" r:id="rId2"/>
     <sheet name="objetos" sheetId="2" r:id="rId3"/>
-    <sheet name="descripciones" sheetId="3" r:id="rId4"/>
-    <sheet name="monstruos" sheetId="4" r:id="rId5"/>
+    <sheet name="obj desc" sheetId="3" r:id="rId4"/>
+    <sheet name="obj_categoria" sheetId="7" r:id="rId5"/>
+    <sheet name="clases" sheetId="9" r:id="rId6"/>
+    <sheet name="rareza" sheetId="8" r:id="rId7"/>
+    <sheet name="castigos" sheetId="11" r:id="rId8"/>
+    <sheet name="monstruos" sheetId="4" r:id="rId9"/>
+    <sheet name="nombres" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="318">
   <si>
     <t>Español</t>
   </si>
@@ -219,12 +224,6 @@
     <t>Fairy</t>
   </si>
   <si>
-    <t>Recover 10 HP points.</t>
-  </si>
-  <si>
-    <t>Recover 20 HP points.</t>
-  </si>
-  <si>
     <t>Join it with other objects, maybe you can get something done.</t>
   </si>
   <si>
@@ -531,15 +530,6 @@
     <t>Fada</t>
   </si>
   <si>
-    <t>No puedes silenciar a un administrador.</t>
-  </si>
-  <si>
-    <t>You cannot mute an administrator.</t>
-  </si>
-  <si>
-    <t>Você não pode silenciar um administrador</t>
-  </si>
-  <si>
     <t>Para silenciar a un moderador tienes que tener permisos de administrador.</t>
   </si>
   <si>
@@ -616,6 +606,396 @@
   </si>
   <si>
     <t>Ter sido avisado {cant} vezes em menos de {tiempo} {medida}.</t>
+  </si>
+  <si>
+    <t>Baneado</t>
+  </si>
+  <si>
+    <t>Fue baneado por:</t>
+  </si>
+  <si>
+    <t>Banned</t>
+  </si>
+  <si>
+    <t>Was banned by:</t>
+  </si>
+  <si>
+    <t>Banido</t>
+  </si>
+  <si>
+    <t>Foi banido por:</t>
+  </si>
+  <si>
+    <t>El parametro &lt;tiempo&gt; debe ser un número entero.</t>
+  </si>
+  <si>
+    <t>The &lt;time&gt; parameter must be an integer.</t>
+  </si>
+  <si>
+    <t>O parâmetro &lt;tempo&gt; deve ser um número inteiro.</t>
+  </si>
+  <si>
+    <t>No puedes silenciar, advertir, banear o expulsar  a un administrador.</t>
+  </si>
+  <si>
+    <t>Você não pode silenciar, avisar, banir ou chutar um administrador.</t>
+  </si>
+  <si>
+    <t>You cannot mute, warn, ban or kick an administrator.</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Nickname</t>
+  </si>
+  <si>
+    <t>Gorfyx (Falso)</t>
+  </si>
+  <si>
+    <t>(Nombre Generico)</t>
+  </si>
+  <si>
+    <t>Hmmmm</t>
+  </si>
+  <si>
+    <t>&amp;@$#/°!*</t>
+  </si>
+  <si>
+    <t>Nombre invalido</t>
+  </si>
+  <si>
+    <t>Alastor</t>
+  </si>
+  <si>
+    <t>NicoCore (Falso)</t>
+  </si>
+  <si>
+    <t>Sospechoso</t>
+  </si>
+  <si>
+    <t>Tengo nuevo nombre</t>
+  </si>
+  <si>
+    <t>Soy fan</t>
+  </si>
+  <si>
+    <t>Nuevo Miembro</t>
+  </si>
+  <si>
+    <t>Caballero</t>
+  </si>
+  <si>
+    <t>Cebolinha</t>
+  </si>
+  <si>
+    <t>Monica</t>
+  </si>
+  <si>
+    <t>Cascão</t>
+  </si>
+  <si>
+    <t>Magali</t>
+  </si>
+  <si>
+    <t>Cosmo</t>
+  </si>
+  <si>
+    <t>Timmy</t>
+  </si>
+  <si>
+    <t>Wanda</t>
+  </si>
+  <si>
+    <t>Tommy</t>
+  </si>
+  <si>
+    <t>Tomas (Chu Chu)</t>
+  </si>
+  <si>
+    <t>Dora</t>
+  </si>
+  <si>
+    <t>Botas</t>
+  </si>
+  <si>
+    <t>Pikachu</t>
+  </si>
+  <si>
+    <t>Pablo</t>
+  </si>
+  <si>
+    <t>Uniqua</t>
+  </si>
+  <si>
+    <t>Tyrone</t>
+  </si>
+  <si>
+    <t>Tasha</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>Walter</t>
+  </si>
+  <si>
+    <t>S.A.N.S. Universe</t>
+  </si>
+  <si>
+    <t>Hollow</t>
+  </si>
+  <si>
+    <t>Mee6 (No te ayudaré)</t>
+  </si>
+  <si>
+    <t>Pterodáctilo</t>
+  </si>
+  <si>
+    <t>Ya sé lo que vamos hacer hoy</t>
+  </si>
+  <si>
+    <t>Pueblerino</t>
+  </si>
+  <si>
+    <t>Crash</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>Fundy (Sin ideas)</t>
+  </si>
+  <si>
+    <t>Dream</t>
+  </si>
+  <si>
+    <t>Felps (Ey ta po-)</t>
+  </si>
+  <si>
+    <t>Celulabit</t>
+  </si>
+  <si>
+    <t>A Cookie (click it)</t>
+  </si>
+  <si>
+    <t>Isaac</t>
+  </si>
+  <si>
+    <t>Alva el majo</t>
+  </si>
+  <si>
+    <t>Guinxu</t>
+  </si>
+  <si>
+    <t>Daarick</t>
+  </si>
+  <si>
+    <t>Hornet</t>
+  </si>
+  <si>
+    <t>Pálido</t>
+  </si>
+  <si>
+    <t>Azucarilla (Quema eso)</t>
+  </si>
+  <si>
+    <t>Caboby</t>
+  </si>
+  <si>
+    <t>Hey, Listen</t>
+  </si>
+  <si>
+    <t>Quirrel</t>
+  </si>
+  <si>
+    <t>Zote</t>
+  </si>
+  <si>
+    <t>Yellow Guy</t>
+  </si>
+  <si>
+    <t>Red Guy</t>
+  </si>
+  <si>
+    <t>Henry (made with sticks)</t>
+  </si>
+  <si>
+    <t>Duck</t>
+  </si>
+  <si>
+    <t>ROY (creador de discord)</t>
+  </si>
+  <si>
+    <t>Grimm</t>
+  </si>
+  <si>
+    <t>Blue Baby</t>
+  </si>
+  <si>
+    <t>Dr.Flug</t>
+  </si>
+  <si>
+    <t>Cyan (🍆land)</t>
+  </si>
+  <si>
+    <t>Grillby</t>
+  </si>
+  <si>
+    <t>Guppy</t>
+  </si>
+  <si>
+    <t>Ari</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Recover 10 HP.</t>
+  </si>
+  <si>
+    <t>Recover 20 HP.</t>
+  </si>
+  <si>
+    <t>Arma</t>
+  </si>
+  <si>
+    <t>Armadura</t>
+  </si>
+  <si>
+    <t>Curación</t>
+  </si>
+  <si>
+    <t>Daño</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Heal</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Curação</t>
+  </si>
+  <si>
+    <t>Dano</t>
+  </si>
+  <si>
+    <t>Muy común</t>
+  </si>
+  <si>
+    <t>Común</t>
+  </si>
+  <si>
+    <t>Poco común</t>
+  </si>
+  <si>
+    <t>Raro</t>
+  </si>
+  <si>
+    <t>Muy raro</t>
+  </si>
+  <si>
+    <t>C̪ͫ͠ó̷̮r̶̩͆r͉ͦ́uͦ̌͏̼̟͝p̶̵̙͕͌̑t̢̡̠̳̔̍a̸̸̲̭ͤ͐</t>
+  </si>
+  <si>
+    <t>Lengendario</t>
+  </si>
+  <si>
+    <t>Very common</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>uncommon</t>
+  </si>
+  <si>
+    <t>Rare</t>
+  </si>
+  <si>
+    <t>Very rare</t>
+  </si>
+  <si>
+    <t>Legendary</t>
+  </si>
+  <si>
+    <t>Ć̹̥ͯ́̀ǫ͍͚͋̊́r̡̖̞̊ͨ̕r̴̠̣̄̉͞u̴̺̮ͯ̓͠p͔̦̆ͬ́͢t͎͙ͧ̀͘͡</t>
+  </si>
+  <si>
+    <t>Sólo dado por admins o eventos</t>
+  </si>
+  <si>
+    <t>Only given by admins or events</t>
+  </si>
+  <si>
+    <t>Muito comum</t>
+  </si>
+  <si>
+    <t>Comum</t>
+  </si>
+  <si>
+    <t>Pouco comum</t>
+  </si>
+  <si>
+    <t>Esquisito</t>
+  </si>
+  <si>
+    <t>Muito esquisito</t>
+  </si>
+  <si>
+    <t>Lendário</t>
+  </si>
+  <si>
+    <t>Ć̷̲̦͆͘o̸̟͖̍ͯ͠r̽ͣ͏̦̙͠r̢̰̩̆̌͝ȍ̢̦̥͒̕m̔̍͏̯̩͝p͙̫ͦͪ̀̕i͔̗͑ͣ͘͢d͕̼͒̿̕͜ǫ̩͈̈́̇͘</t>
+  </si>
+  <si>
+    <t>Só pode ser obtido por administradores ou eventos</t>
+  </si>
+  <si>
+    <t>Enseñanza</t>
+  </si>
+  <si>
+    <t>Teaching</t>
+  </si>
+  <si>
+    <t>Ensinança</t>
+  </si>
+  <si>
+    <t>Aumento de estadistica</t>
+  </si>
+  <si>
+    <t>Stat boost</t>
+  </si>
+  <si>
+    <t>Aumento de estadística</t>
+  </si>
+  <si>
+    <t>Cavaleiro</t>
+  </si>
+  <si>
+    <t>Knight</t>
+  </si>
+  <si>
+    <t>Silenciar</t>
+  </si>
+  <si>
+    <t>Baneo temporal</t>
+  </si>
+  <si>
+    <t>Expulsar</t>
+  </si>
+  <si>
+    <t>Baneo</t>
   </si>
 </sst>
 </file>
@@ -672,7 +1052,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -683,6 +1063,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Énfasis6" xfId="1" builtinId="49"/>
@@ -998,10 +1379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECE8E95-8ADA-4BBB-8313-6E88F6DAFB67}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,7 +1398,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1031,7 +1412,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1045,7 +1426,7 @@
         <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1059,7 +1440,7 @@
         <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1067,13 +1448,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1087,7 +1468,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1101,7 +1482,7 @@
         <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1109,13 +1490,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1143,7 +1524,7 @@
         <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1157,7 +1538,7 @@
         <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1171,7 +1552,7 @@
         <v>33</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1185,7 +1566,7 @@
         <v>34</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1196,10 +1577,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1213,7 +1594,7 @@
         <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1224,10 +1605,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1235,13 +1616,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1249,13 +1630,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1269,7 +1650,7 @@
         <v>37</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1283,7 +1664,7 @@
         <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1297,7 +1678,7 @@
         <v>39</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1311,7 +1692,7 @@
         <v>40</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1339,7 +1720,7 @@
         <v>42</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1353,7 +1734,7 @@
         <v>43</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1367,7 +1748,7 @@
         <v>44</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1381,7 +1762,7 @@
         <v>45</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1395,7 +1776,7 @@
         <v>46</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1403,13 +1784,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1417,13 +1798,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1431,13 +1812,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1445,13 +1826,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1459,13 +1840,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1473,13 +1854,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1487,13 +1868,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1501,13 +1882,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1515,13 +1896,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1529,13 +1910,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1543,13 +1924,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1557,13 +1938,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1571,27 +1952,27 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1599,13 +1980,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1613,13 +1994,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1627,13 +2008,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1641,13 +2022,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1655,13 +2036,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1669,13 +2050,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1683,13 +2064,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1697,13 +2078,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1711,27 +2092,443 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>192</v>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D75ED0-03EE-4F5F-A8FA-A4B195E7A751}">
+  <dimension ref="A1:A71"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -1745,7 +2542,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1761,21 +2558,21 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1788,7 +2585,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1805,26 +2602,26 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>48</v>
@@ -1833,32 +2630,32 @@
         <v>57</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>50</v>
@@ -1866,44 +2663,44 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1917,7 +2714,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1933,105 +2730,105 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>60</v>
+        <v>270</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>61</v>
+        <v>271</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2040,11 +2837,420 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A0FDCD-7B01-49CC-8833-80CF878A1603}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>306</v>
+      </c>
+      <c r="C6" t="s">
+        <v>307</v>
+      </c>
+      <c r="D6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>309</v>
+      </c>
+      <c r="C7" t="s">
+        <v>310</v>
+      </c>
+      <c r="D7" t="s">
+        <v>311</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4CF48A-E7C7-43BD-935D-6B321CCFD5AD}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2FD0E4E-F9D5-425C-9548-AD62BC922F02}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" t="s">
+        <v>293</v>
+      </c>
+      <c r="D6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>288</v>
+      </c>
+      <c r="C7" t="s">
+        <v>294</v>
+      </c>
+      <c r="D7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C8" t="s">
+        <v>295</v>
+      </c>
+      <c r="D8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>296</v>
+      </c>
+      <c r="C9" t="s">
+        <v>297</v>
+      </c>
+      <c r="D9" t="s">
+        <v>305</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E33FD6-CA65-45FC-99DF-76FACBB08E47}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9572496D-EE77-4B6C-AC88-9EA6DD028EAC}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2060,12 +3266,12 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>57</v>
@@ -2079,7 +3285,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>58</v>
@@ -2088,7 +3294,7 @@
         <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rediseño de base de datos 0.3
</commit_message>
<xml_diff>
--- a/cogs/idiomas.xlsx
+++ b/cogs/idiomas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Proyecto bot de Discord\Codigo\cogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60266F42-2E24-4B06-9B56-500F238FDDA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA4E602-AC7D-48B1-80EB-79991E2521FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DE6446BD-563B-4FC6-AA1A-933AD8BD7CBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{DE6446BD-563B-4FC6-AA1A-933AD8BD7CBF}"/>
   </bookViews>
   <sheets>
     <sheet name="bot" sheetId="1" r:id="rId1"/>
@@ -992,10 +992,10 @@
     <t>Baneo temporal</t>
   </si>
   <si>
-    <t>Expulsar</t>
-  </si>
-  <si>
     <t>Baneo</t>
+  </si>
+  <si>
+    <t>Explusar</t>
   </si>
 </sst>
 </file>
@@ -1381,7 +1381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECE8E95-8ADA-4BBB-8313-6E88F6DAFB67}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
@@ -3188,8 +3188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E33FD6-CA65-45FC-99DF-76FACBB08E47}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3221,7 +3221,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3229,7 +3229,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3237,7 +3237,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rediseño de base de datos 0.4
</commit_message>
<xml_diff>
--- a/cogs/idiomas.xlsx
+++ b/cogs/idiomas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Proyecto bot de Discord\Codigo\cogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA4E602-AC7D-48B1-80EB-79991E2521FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68148641-AADD-4B3E-9908-5E790BA69FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{DE6446BD-563B-4FC6-AA1A-933AD8BD7CBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DE6446BD-563B-4FC6-AA1A-933AD8BD7CBF}"/>
   </bookViews>
   <sheets>
     <sheet name="bot" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="308">
   <si>
     <t>Español</t>
   </si>
@@ -548,33 +548,12 @@
     <t>A palavra ||{palabra}|| é proibida neste servidor.</t>
   </si>
   <si>
-    <t>Moderador</t>
-  </si>
-  <si>
-    <t>Moderator</t>
-  </si>
-  <si>
-    <t>Silenciado</t>
-  </si>
-  <si>
-    <t>Muted</t>
-  </si>
-  <si>
-    <t>Fue silenciado por:</t>
-  </si>
-  <si>
-    <t>Foi silenciado por:</t>
-  </si>
-  <si>
     <t>Usuario:</t>
   </si>
   <si>
     <t>User:</t>
   </si>
   <si>
-    <t>Was silenced by:</t>
-  </si>
-  <si>
     <t>Reason:</t>
   </si>
   <si>
@@ -584,48 +563,12 @@
     <t>Razão:</t>
   </si>
   <si>
-    <t>Warned</t>
-  </si>
-  <si>
-    <t>Avisado</t>
-  </si>
-  <si>
-    <t>Fue avisado por:</t>
-  </si>
-  <si>
-    <t>Was warned by:</t>
-  </si>
-  <si>
-    <t>Foi avisado por:</t>
-  </si>
-  <si>
-    <t>Haber sido avisado {cant} veces en menos de {tiempo} {medida}.</t>
-  </si>
-  <si>
     <t>Having been warned {cant} times in less than {tiempo} {medida}.</t>
   </si>
   <si>
     <t>Ter sido avisado {cant} vezes em menos de {tiempo} {medida}.</t>
   </si>
   <si>
-    <t>Baneado</t>
-  </si>
-  <si>
-    <t>Fue baneado por:</t>
-  </si>
-  <si>
-    <t>Banned</t>
-  </si>
-  <si>
-    <t>Was banned by:</t>
-  </si>
-  <si>
-    <t>Banido</t>
-  </si>
-  <si>
-    <t>Foi banido por:</t>
-  </si>
-  <si>
     <t>El parametro &lt;tiempo&gt; debe ser un número entero.</t>
   </si>
   <si>
@@ -986,16 +929,43 @@
     <t>Knight</t>
   </si>
   <si>
-    <t>Silenciar</t>
-  </si>
-  <si>
-    <t>Baneo temporal</t>
-  </si>
-  <si>
-    <t>Baneo</t>
-  </si>
-  <si>
-    <t>Explusar</t>
+    <t>silenciado</t>
+  </si>
+  <si>
+    <t>baneado temporalmente</t>
+  </si>
+  <si>
+    <t>expulsado</t>
+  </si>
+  <si>
+    <t>baneado</t>
+  </si>
+  <si>
+    <t>**[AVISO]**</t>
+  </si>
+  <si>
+    <t>**[CASTIGO]**</t>
+  </si>
+  <si>
+    <t>Mensaje:</t>
+  </si>
+  <si>
+    <t>Información:</t>
+  </si>
+  <si>
+    <t>El miembro {member} ha sido {castigo} por el moderador {mod}</t>
+  </si>
+  <si>
+    <t>avisado</t>
+  </si>
+  <si>
+    <t>Haber sido avisado 1 vez en menos de {tiempo}.</t>
+  </si>
+  <si>
+    <t>Haber sido avisado {cant} veces en menos de {tiempo}.</t>
+  </si>
+  <si>
+    <t>Duración del castigo:</t>
   </si>
 </sst>
 </file>
@@ -1381,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECE8E95-8ADA-4BBB-8313-6E88F6DAFB67}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1966,13 +1936,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2003,18 +1973,12 @@
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>168</v>
+        <v>303</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2022,13 +1986,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>170</v>
+        <v>299</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2036,13 +1994,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>173</v>
+        <v>300</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2050,13 +2002,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>181</v>
+        <v>301</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2064,13 +2010,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2078,27 +2024,27 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>189</v>
+        <v>306</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2106,13 +2052,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>174</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2120,27 +2060,21 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C53" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>187</v>
+        <v>302</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2148,13 +2082,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>196</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -2178,202 +2106,202 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
@@ -2383,152 +2311,152 @@
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>254</v>
+        <v>235</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>261</v>
+        <v>242</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>266</v>
+        <v>247</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>268</v>
+        <v>249</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>269</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2741,7 +2669,7 @@
         <v>151</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>152</v>
@@ -2769,7 +2697,7 @@
         <v>154</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>271</v>
+        <v>252</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>155</v>
@@ -2865,13 +2793,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
       <c r="C2" t="s">
-        <v>276</v>
+        <v>257</v>
       </c>
       <c r="D2" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2879,13 +2807,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>273</v>
+        <v>254</v>
       </c>
       <c r="C3" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="D3" t="s">
-        <v>273</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2893,13 +2821,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>274</v>
+        <v>255</v>
       </c>
       <c r="C4" t="s">
-        <v>278</v>
+        <v>259</v>
       </c>
       <c r="D4" t="s">
-        <v>280</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2907,13 +2835,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>275</v>
+        <v>256</v>
       </c>
       <c r="C5" t="s">
-        <v>279</v>
+        <v>260</v>
       </c>
       <c r="D5" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2921,13 +2849,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>306</v>
+        <v>287</v>
       </c>
       <c r="C6" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
       <c r="D6" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2935,13 +2863,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
       <c r="C7" t="s">
-        <v>310</v>
+        <v>291</v>
       </c>
       <c r="D7" t="s">
-        <v>311</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2979,13 +2907,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="C2" t="s">
-        <v>313</v>
+        <v>294</v>
       </c>
       <c r="D2" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3072,13 +3000,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
       <c r="C2" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="D2" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3086,13 +3014,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="C3" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
       <c r="D3" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3100,13 +3028,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="C4" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="D4" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3114,13 +3042,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="C5" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="D5" t="s">
-        <v>301</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3128,13 +3056,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="C6" t="s">
-        <v>293</v>
+        <v>274</v>
       </c>
       <c r="D6" t="s">
-        <v>302</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3142,13 +3070,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>288</v>
+        <v>269</v>
       </c>
       <c r="C7" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="D7" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3156,13 +3084,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
       <c r="C8" t="s">
-        <v>295</v>
+        <v>276</v>
       </c>
       <c r="D8" t="s">
-        <v>304</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3170,13 +3098,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="C9" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="D9" t="s">
-        <v>305</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -3186,10 +3114,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E33FD6-CA65-45FC-99DF-76FACBB08E47}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3210,34 +3138,42 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>317</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>316</v>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>